<commit_message>
Delete duplicate entry for Woodford
</commit_message>
<xml_diff>
--- a/data_folder/child_nutrition/child_meals_2019.xlsx
+++ b/data_folder/child_nutrition/child_meals_2019.xlsx
@@ -424,12 +424,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -452,8 +456,8 @@
   </sheetPr>
   <dimension ref="A1:E104"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A84" activeCellId="0" sqref="A84"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A83" activeCellId="0" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1601,8 +1605,8 @@
         <v>2334</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B83" s="0" t="n">

</xml_diff>

<commit_message>
Properly cleared last row
</commit_message>
<xml_diff>
--- a/data_folder/child_nutrition/child_meals_2019.xlsx
+++ b/data_folder/child_nutrition/child_meals_2019.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
   <si>
     <t xml:space="preserve">County</t>
   </si>
@@ -424,16 +424,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -457,7 +453,7 @@
   <dimension ref="A1:E104"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A83" activeCellId="0" sqref="A83"/>
+      <selection pane="topLeft" activeCell="A104" activeCellId="0" sqref="104:104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1605,8 +1601,8 @@
         <v>2334</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="2" t="s">
+    <row r="83" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
         <v>86</v>
       </c>
       <c r="B83" s="0" t="n">
@@ -1908,14 +1904,7 @@
         <v>1778</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="B104" s="0" t="n">
-        <v>229499</v>
-      </c>
-    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>